<commit_message>
:tada: Don't extract from hidden xlsx sheets
[master]
</commit_message>
<xml_diff>
--- a/test/fixtures/test_xlsx.xlsx
+++ b/test/fixtures/test_xlsx.xlsx
@@ -1,41 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21320"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3C5E978-C066-41A0-BA18-C665A90C2137}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weilandia/workspace/simple_text_extract/test/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF126247-A86F-554D-86A8-840BA9B48C00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="14800" windowHeight="8020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ruby</t>
   </si>
   <si>
     <t>js</t>
   </si>
+  <si>
+    <t>This sheet is hidden.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,13 +384,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,13 +407,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30732E7-587B-4966-867E-92F41735B9FF}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{C2EB2F4B-8EA2-5222-905D-68FF1D667B20}">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -422,4 +424,22 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5C552F3-6414-CA49-97DD-7D6F39ECC2D1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>